<commit_message>
Fixed the following issues - tempates were in utf-8-bom instead of just utf-8 - changed template line endings from LF to CRLF
Review.html --> more ajax work
- have delete functionality working
- have multi-delete mostly working
- still need to work on adding a new row or item

To Do:
- upload view --> need to change logic on a reupload (delete everything for that month/year) and reload the data
- review.html --> add a row correctly
- get totals going correctly
</commit_message>
<xml_diff>
--- a/django-base/charmsapp/xlsx_files/SampleDataExcel.xlsx
+++ b/django-base/charmsapp/xlsx_files/SampleDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\source\repos\SMarhefka\IS601\django-base\charmsapp\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F48C43-2AAD-4F43-8949-CCC81246F452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43709CC3-80BB-404F-A119-466B6FC16078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CEE0D2C-EBA8-484A-BFFA-9525299E0D72}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>first name</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Lana</t>
   </si>
 </sst>
 </file>
@@ -140,12 +146,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -462,9 +471,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E04D5F-B6CF-4BCE-AAEC-8222152B64BF}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -490,7 +501,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -499,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="E2" s="3">
         <v>43882</v>
@@ -556,14 +567,41 @@
         <v>43941</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>77</v>
+      </c>
+      <c r="E7" s="3">
+        <v>43882</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{98C87A5E-B1F1-4259-B5F7-FA358D23634E}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{21978BAB-7F7D-403B-87DE-6AC03E590AED}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{12A72E9C-698F-4DD2-9D7D-D148AD99B551}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{33505615-406C-4F5B-B123-460A10EDC9DE}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{6604878A-8293-4428-926B-AF1238125FA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>